<commit_message>
Added new references for ATH, maize, rice and tomato on top of dropdown
</commit_message>
<xml_diff>
--- a/www/input_data/TableForReferenceScData_11072023.xlsx
+++ b/www/input_data/TableForReferenceScData_11072023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saipavanbathala/Documents/Li_Lab/OMGBrowser/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sai/Vtech/Li_Lab/OMGBrowser/www/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77455EC-5F6E-C148-A6A7-0905DEDF9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0031FA7-0063-4B4D-A058-E54A260FEF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="94">
   <si>
     <t>Reference File Name</t>
   </si>
@@ -291,13 +291,40 @@
   </si>
   <si>
     <t>MtrunA17r5</t>
+  </si>
+  <si>
+    <t>Arabidopsis</t>
+  </si>
+  <si>
+    <t>ATH****</t>
+  </si>
+  <si>
+    <t>Ptrichocarpa</t>
+  </si>
+  <si>
+    <t>Potri.001G134900.1.p</t>
+  </si>
+  <si>
+    <t>Solanum_lycopersicum_1(new).csv</t>
+  </si>
+  <si>
+    <t>Arabidopsis_1(new).csv</t>
+  </si>
+  <si>
+    <t>Zeamays_1(new).csv</t>
+  </si>
+  <si>
+    <t>Oryza_1(new).csv</t>
+  </si>
+  <si>
+    <t>Zeamays</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -310,6 +337,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -332,8 +365,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ABD0FC-1E3D-C049-90D3-7F47A0518D42}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="223" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,22 +728,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
         <v>61</v>
@@ -717,25 +754,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
         <v>61</v>
@@ -743,77 +780,77 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
         <v>61</v>
@@ -821,25 +858,25 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
         <v>61</v>
@@ -847,77 +884,77 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
         <v>76</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
         <v>61</v>
@@ -931,7 +968,7 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>52</v>
@@ -943,7 +980,7 @@
         <v>76</v>
       </c>
       <c r="G11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
         <v>61</v>
@@ -957,7 +994,7 @@
         <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>52</v>
@@ -969,7 +1006,7 @@
         <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
         <v>61</v>
@@ -977,25 +1014,25 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
         <v>61</v>
@@ -1003,25 +1040,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
         <v>61</v>
@@ -1029,25 +1066,25 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
         <v>61</v>
@@ -1055,25 +1092,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H16" t="s">
         <v>61</v>
@@ -1081,22 +1118,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
         <v>76</v>
@@ -1107,22 +1144,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
         <v>76</v>
@@ -1133,22 +1170,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G19" t="s">
         <v>76</v>
@@ -1159,28 +1196,158 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="s">
         <v>78</v>
       </c>
-      <c r="H20" t="s">
-        <v>61</v>
+      <c r="H24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the excel file.
</commit_message>
<xml_diff>
--- a/www/input_data/TableForReferenceScData_11072023.xlsx
+++ b/www/input_data/TableForReferenceScData_11072023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sai/Vtech/Li_Lab/OMGBrowser/www/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/songli_vt_edu/Documents/A_NinaProjects_2022/SingleCellCrossSpecies_2022/OMGbrowser_Final_11132023/OMGBrowser/www/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0031FA7-0063-4B4D-A058-E54A260FEF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
+    <workbookView xWindow="6320" yWindow="2200" windowWidth="28800" windowHeight="15800" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ABD0FC-1E3D-C049-90D3-7F47A0518D42}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="223" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added new Orthomarker.tsv, changed input file list xlsx file
</commit_message>
<xml_diff>
--- a/www/input_data/TableForReferenceScData_11072023.xlsx
+++ b/www/input_data/TableForReferenceScData_11072023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/songli_vt_edu/Documents/A_NinaProjects_2022/SingleCellCrossSpecies_2022/OMGbrowser_Final_11132023/OMGBrowser/www/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/songli_vt_edu/Documents/A_NinaProjects_2022/SingleCellCrossSpecies_2022/OMGBrowser_NinaNewVersion_12-21-2023/OMGBrowser/www/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0031FA7-0063-4B4D-A058-E54A260FEF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708D97EE-442B-2A48-8A24-092F90C9BC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="2200" windowWidth="28800" windowHeight="15800" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
+    <workbookView xWindow="6500" yWindow="1400" windowWidth="28800" windowHeight="15900" xr2:uid="{C17EE9DD-9FFE-464F-B37F-5C4FA6E87D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
   <si>
     <t>Reference File Name</t>
   </si>
@@ -95,30 +95,15 @@
     <t>Single-cell RNA sequencing provides a high-resolution roadmap for understanding the multicellular compartmentation of specialized metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Oryza_1(leaf).csv </t>
-  </si>
-  <si>
     <t>10.3389/fpls.2020.603302</t>
   </si>
   <si>
-    <t>10.1111/nph.18008</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fragaria_vesca_1(Unknown).csv </t>
   </si>
   <si>
     <t>10.1038/s41467-021-22352-4</t>
   </si>
   <si>
-    <t>10.1016/j.molp.2020.12.014</t>
-  </si>
-  <si>
-    <t>10.1016/j.devcel.2023.03.004</t>
-  </si>
-  <si>
-    <t>10.1016/j.jgg.2021.06.001</t>
-  </si>
-  <si>
     <t xml:space="preserve">Populus_alba_var_pyramidalis_1(stem).csv </t>
   </si>
   <si>
@@ -131,15 +116,6 @@
     <t xml:space="preserve">Gossypium_hirsutum_1(Ovule outer integument).csv  </t>
   </si>
   <si>
-    <t xml:space="preserve">Solanum_lycopersicum_1(root).csv </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MtrunA17r5_1(root).csv  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solanum_lycopersicum_2(root).csv </t>
-  </si>
-  <si>
     <t>10.1093/hr/uhab055</t>
   </si>
   <si>
@@ -197,21 +173,9 @@
     <t>?</t>
   </si>
   <si>
-    <t>PRJNA868047</t>
-  </si>
-  <si>
-    <t>Cell-specific pathways recruited for symbiotic nodulation in the Medicago truncatula legume</t>
-  </si>
-  <si>
-    <t>10.1016/j.molp.2022.10.021</t>
-  </si>
-  <si>
     <t>Gene Pattern</t>
   </si>
   <si>
-    <t>BRA****</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -227,54 +191,21 @@
     <t>No</t>
   </si>
   <si>
-    <t>NIC***</t>
-  </si>
-  <si>
     <t>Nicotiana_attenuata</t>
   </si>
   <si>
     <t>Reference_Available</t>
   </si>
   <si>
-    <t>Oryza_indica</t>
-  </si>
-  <si>
-    <t>BGIOSGA002439</t>
-  </si>
-  <si>
     <t>Solyc02g079570</t>
   </si>
   <si>
-    <t>Os03t0556600</t>
-  </si>
-  <si>
-    <t>Oryza</t>
-  </si>
-  <si>
-    <t>Os03t0556601</t>
-  </si>
-  <si>
-    <t>Os03t0556602</t>
-  </si>
-  <si>
-    <t>Os03t0556603</t>
-  </si>
-  <si>
-    <t>Os03t0556604</t>
-  </si>
-  <si>
-    <t>Os03t0556605</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>Catharanthus_roseus</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Fragaria_vesca</t>
   </si>
   <si>
@@ -290,41 +221,131 @@
     <t>Gossypium_hirsutum</t>
   </si>
   <si>
-    <t>MtrunA17r5</t>
-  </si>
-  <si>
-    <t>Arabidopsis</t>
-  </si>
-  <si>
-    <t>ATH****</t>
-  </si>
-  <si>
-    <t>Ptrichocarpa</t>
-  </si>
-  <si>
-    <t>Potri.001G134900.1.p</t>
-  </si>
-  <si>
-    <t>Solanum_lycopersicum_1(new).csv</t>
-  </si>
-  <si>
-    <t>Arabidopsis_1(new).csv</t>
-  </si>
-  <si>
-    <t>Zeamays_1(new).csv</t>
-  </si>
-  <si>
-    <t>Oryza_1(new).csv</t>
-  </si>
-  <si>
-    <t>Zeamays</t>
+    <t>Arabidopsis_thaliana</t>
+  </si>
+  <si>
+    <t>10.1104/pp.18.01482</t>
+  </si>
+  <si>
+    <t>GSE123013</t>
+  </si>
+  <si>
+    <t>Single-Cell RNA Sequencing Resolves Molecular Relationships Among Individual Plant Cells</t>
+  </si>
+  <si>
+    <t>Oryza_sativa</t>
+  </si>
+  <si>
+    <t>PRJNA706435</t>
+  </si>
+  <si>
+    <t>Single-cell transcriptome atlas and chromatin accessibility landscape reveal differentiation trajectories in the rice root</t>
+  </si>
+  <si>
+    <t>A suberized exodermis is required for tomato drought tolerance</t>
+  </si>
+  <si>
+    <t>10.1101/2022.10.10.511665</t>
+  </si>
+  <si>
+    <t>GSE212405</t>
+  </si>
+  <si>
+    <t>10.1101/2021.04.28.441892</t>
+  </si>
+  <si>
+    <t>Ground tissue circuitry regulates organ complexity in cereal roots</t>
+  </si>
+  <si>
+    <t>Single-nucleus RNA-seq resolves spatiotemporal developmental trajectories in the tomato shoot apex</t>
+  </si>
+  <si>
+    <t>10.1101/2020.09.20.305029</t>
+  </si>
+  <si>
+    <t>SAMN16069893</t>
+  </si>
+  <si>
+    <t>10.1016/j.devcel.2021.02.021</t>
+  </si>
+  <si>
+    <t>A single-cell analysis of the Arabidopsis vegetative shoot apex</t>
+  </si>
+  <si>
+    <t>PRJCA003094</t>
+  </si>
+  <si>
+    <t>Os03g0556600</t>
+  </si>
+  <si>
+    <t>AT1G11280</t>
+  </si>
+  <si>
+    <t>Zm00001d002173</t>
+  </si>
+  <si>
+    <t>Bra000261</t>
+  </si>
+  <si>
+    <t>FvH4_3g03230</t>
+  </si>
+  <si>
+    <t>A4A49_01158</t>
+  </si>
+  <si>
+    <t>M9H77_34801</t>
+  </si>
+  <si>
+    <t>Gbi01G2078</t>
+  </si>
+  <si>
+    <t>Pop_A01G017586</t>
+  </si>
+  <si>
+    <t>Ghir_A01G003270</t>
+  </si>
+  <si>
+    <t>pal_pou00430</t>
+  </si>
+  <si>
+    <t>Potri_001G134900</t>
+  </si>
+  <si>
+    <t>Arabidopsis_thaliana_3(Root).csv</t>
+  </si>
+  <si>
+    <t>Arabidopsis_thaliana_3(Shoot axis apex).csv</t>
+  </si>
+  <si>
+    <t>Oryza_sativa_3(Root).csv</t>
+  </si>
+  <si>
+    <t>Solanum_lycopersicum_3(Root).csv</t>
+  </si>
+  <si>
+    <t>Solanum_lycopersicum_3(Shoot).csv</t>
+  </si>
+  <si>
+    <t>Zea_mays_3(Root).csv</t>
+  </si>
+  <si>
+    <t>Zea_mays</t>
+  </si>
+  <si>
+    <t>Populus_trichocarpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oryza_sativa_1(leaf).csv </t>
+  </si>
+  <si>
+    <t>Populus_trichocarpa_3(Shoot).csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -337,12 +358,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -365,9 +380,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ABD0FC-1E3D-C049-90D3-7F47A0518D42}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="223" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -720,440 +734,428 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
         <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1162,196 +1164,20 @@
         <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" t="s">
-        <v>76</v>
-      </c>
-      <c r="H23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/Traces/study/?acc=PRJNA706435" xr:uid="{4D291742-D5F9-EB41-9286-B1FAEB32AEC1}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://doi.org/10.1038/s41467-021-22352-4" xr:uid="{4C419606-BE67-B846-BF3C-B440D677E712}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://www.biorxiv.org/content/10.1101/2022.10.10.511665.abstract" xr:uid="{120902BF-B1D8-3B4C-9384-33AE91DD50D9}"/>
+    <hyperlink ref="C6" r:id="rId4" display="https://doi.org/10.1016/j.devcel.2021.02.021" xr:uid="{9798EF2E-762C-934D-AE0F-0D9FCB060BAF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>